<commit_message>
fixed hollys name in 4019
</commit_message>
<xml_diff>
--- a/library/library_4019.xlsx
+++ b/library/library_4019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="31">
   <si>
     <t xml:space="preserve">s2cDNADate</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">08.14.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H.BROWN</t>
   </si>
   <si>
     <t xml:space="preserve">TCCGGGA</t>
@@ -229,7 +232,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:F19"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,13 +283,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>207</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,13 +306,13 @@
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>208</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,13 +329,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>209</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,13 +352,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>210</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,13 +375,13 @@
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>211</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,13 +398,13 @@
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>212</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,13 +421,13 @@
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>213</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,13 +444,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>214</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,13 +467,13 @@
         <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>215</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,13 +490,13 @@
         <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>216</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,13 +513,13 @@
         <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>217</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,13 +536,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>218</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,13 +559,13 @@
         <v>11</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>219</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,13 +582,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>220</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>221</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,13 +628,13 @@
         <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>222</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,13 +651,13 @@
         <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>223</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,13 +674,13 @@
         <v>11</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>224</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continuing to fix name misspelling
</commit_message>
<xml_diff>
--- a/library/library_4019.xlsx
+++ b/library/library_4019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
   <si>
     <t xml:space="preserve">s2cDNADate</t>
   </si>
@@ -52,13 +52,10 @@
     <t xml:space="preserve">07.27.18</t>
   </si>
   <si>
-    <t xml:space="preserve">H.BOWN</t>
+    <t xml:space="preserve">H.BROWN</t>
   </si>
   <si>
     <t xml:space="preserve">08.14.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H.BROWN</t>
   </si>
   <si>
     <t xml:space="preserve">TCCGGGA</t>
@@ -232,7 +229,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E19"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -283,13 +280,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>207</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,13 +303,13 @@
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>208</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,13 +326,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>209</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,13 +349,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>210</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,13 +372,13 @@
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>211</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,13 +395,13 @@
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>212</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,13 +418,13 @@
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>213</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,13 +441,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>214</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,13 +464,13 @@
         <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>215</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,13 +487,13 @@
         <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>216</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,13 +510,13 @@
         <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>217</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,13 +533,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>218</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,13 +556,13 @@
         <v>11</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>219</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,13 +579,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>220</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,13 +602,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>221</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,13 +625,13 @@
         <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>222</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,13 +648,13 @@
         <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>223</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,13 +671,13 @@
         <v>11</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>224</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding library prep protocol to 3569 and 4019, fixing s1cDNAProtocol column in jp 72920
</commit_message>
<xml_diff>
--- a/library/library_4019.xlsx
+++ b/library/library_4019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="32">
   <si>
     <t xml:space="preserve">s2cDNADate</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">index2Sequence</t>
   </si>
   <si>
+    <t xml:space="preserve">libraryProtocol</t>
+  </si>
+  <si>
     <t xml:space="preserve">07.27.18</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">TCCGGGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E7420L</t>
   </si>
   <si>
     <t xml:space="preserve">CGAAAGT</t>
@@ -119,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -147,6 +153,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -200,13 +220,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -226,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B19"/>
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,7 +265,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -265,421 +293,486 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>207</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>207</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>208</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>208</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>209</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>209</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>210</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>210</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>211</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>211</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>212</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>212</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>213</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>213</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>214</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>214</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>215</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>215</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>216</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>216</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>217</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>217</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>218</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>218</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>219</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>219</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>220</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>220</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>221</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>221</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>222</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>222</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>223</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>223</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>224</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>224</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
+        <v>31</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>